<commit_message>
Corrections: - texts corrected in template tables
</commit_message>
<xml_diff>
--- a/app/download_dir/белье_по каждому размеру.xlsx
+++ b/app/download_dir/белье_по каждому размеру.xlsx
@@ -133,7 +133,7 @@
     <t xml:space="preserve">здесь ничего заполнять не нужно,. После внесения всех остальных колонок проверьте правильность заполнения данной колонки, если что то не устраивает то правьте наименование ВРУЧНУЮ. Данная информация будет на этикетке</t>
   </si>
   <si>
-    <t xml:space="preserve">Укажите торговую марку или бренд. Если ничего нет т укажите "Без торгового знака"</t>
+    <t xml:space="preserve">Укажите торговую марку или бренд. Если ничего нет т укажите "Без товарного знака"</t>
   </si>
   <si>
     <t xml:space="preserve">не заполнять</t>
@@ -3222,10 +3222,10 @@
   <dimension ref="A1:AMJ1732"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1658" activeCellId="0" sqref="G1658"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="66.34"/>
@@ -32501,7 +32501,7 @@
       <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50"/>
@@ -34483,7 +34483,7 @@
       <selection pane="topLeft" activeCell="B58" activeCellId="0" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.76"/>

</xml_diff>

<commit_message>
Corrections: - countries edited
</commit_message>
<xml_diff>
--- a/app/download_dir/белье_по каждому размеру.xlsx
+++ b/app/download_dir/белье_по каждому размеру.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2321" uniqueCount="674">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2325" uniqueCount="678">
   <si>
     <t xml:space="preserve">Код ТНВЭД</t>
   </si>
@@ -1257,7 +1257,7 @@
     <t xml:space="preserve">МАЛАВИ</t>
   </si>
   <si>
-    <t xml:space="preserve">МАЛАЙЗИЯ</t>
+    <t xml:space="preserve">МАЛАЙЗИИЯ</t>
   </si>
   <si>
     <t xml:space="preserve">МАЛИ</t>
@@ -1398,10 +1398,13 @@
     <t xml:space="preserve">РЕСПУБЛИКА КОРЕЯ</t>
   </si>
   <si>
+    <t xml:space="preserve">РЕСПУБЛИКА МАКЕДОНИЯ, БЫВШАЯ ЮГОСЛАВСКАЯ РЕСПУБЛИКА</t>
+  </si>
+  <si>
     <t xml:space="preserve">РЕЮНЬОН</t>
   </si>
   <si>
-    <t xml:space="preserve">РОССИЯ</t>
+    <t xml:space="preserve">РОССИЙСКАЯ ФЕДЕРАЦИЯ</t>
   </si>
   <si>
     <t xml:space="preserve">РУАНДА</t>
@@ -1431,13 +1434,7 @@
     <t xml:space="preserve">СЕВЕРНЫЕ МАРИАНСКИЕ ОСТРОВА</t>
   </si>
   <si>
-    <t xml:space="preserve">СЕЙШЕЛЬСКИЕ ОСТРОВА</t>
-  </si>
-  <si>
-    <t xml:space="preserve">СЕН-БАРТЕЛЕМИ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">СЕН-МАРТЕН</t>
+    <t xml:space="preserve">СЕЙШЕЛЬСКИЕ ОСТОРВА</t>
   </si>
   <si>
     <t xml:space="preserve">СЕН-ПЬЕР И МИКЕЛОН</t>
@@ -1449,7 +1446,7 @@
     <t xml:space="preserve">СЕНТ-ВИНСЕНТ И ГРЕНАДИНЫ</t>
   </si>
   <si>
-    <t xml:space="preserve">СЕНТ-КИТС И НЕВИС</t>
+    <t xml:space="preserve">СЕНТ-КИТТС И НЕВИС</t>
   </si>
   <si>
     <t xml:space="preserve">СЕНТ-ЛЮСИЯ</t>
@@ -1461,7 +1458,7 @@
     <t xml:space="preserve">СИНГАПУР</t>
   </si>
   <si>
-    <t xml:space="preserve">СИРИЙСКАЯ АРАБСКАЯ РЕСПУБЛИКА</t>
+    <t xml:space="preserve">СИРИЯ</t>
   </si>
   <si>
     <t xml:space="preserve">СЛОВАКИЯ</t>
@@ -1470,6 +1467,9 @@
     <t xml:space="preserve">СЛОВЕНИЯ</t>
   </si>
   <si>
+    <t xml:space="preserve">СОЕДИНЕННЫЕ ШТАТЫ</t>
+  </si>
+  <si>
     <t xml:space="preserve">СОЛОМОНОВЫ ОСТРОВА</t>
   </si>
   <si>
@@ -1488,13 +1488,16 @@
     <t xml:space="preserve">ТАДЖИКИСТАН</t>
   </si>
   <si>
-    <t xml:space="preserve">ТАЙВАНЬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ТАЙЛАНД</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ТАНЗАНИЯ</t>
+    <t xml:space="preserve">ТАИЛАНД</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТАЙВАНЬ, ПРОВИНЦИЯ КИТАЯ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТАНЗАНИЯ, ОБЪЕДИНЕННАЯ РЕСПУБЛИКА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТЕРКС И КАЙКОС</t>
   </si>
   <si>
     <t xml:space="preserve">ТОГО</t>
@@ -1515,7 +1518,7 @@
     <t xml:space="preserve">ТУНИС</t>
   </si>
   <si>
-    <t xml:space="preserve">ТУРКМЕНИСТАН</t>
+    <t xml:space="preserve">ТУРКМЕНИЯ</t>
   </si>
   <si>
     <t xml:space="preserve">ТУРЦИЯ</t>
@@ -1563,10 +1566,13 @@
     <t xml:space="preserve">ФРАНЦУЗСКИЕ ЮЖНЫЕ ТЕРРИТОРИИ</t>
   </si>
   <si>
+    <t xml:space="preserve">ХЕРДА И МАКДОНАЛЬДА ОСТРОВА</t>
+  </si>
+  <si>
     <t xml:space="preserve">ХОРВАТИЯ</t>
   </si>
   <si>
-    <t xml:space="preserve">ЦЕНТРАЛЬНО-АФРИКАНСКАЯ РЕСПУБЛИКА</t>
+    <t xml:space="preserve">ЦЕНТРАЛЬНОАФРИКАНСКАЯ РЕСПУБЛИКА</t>
   </si>
   <si>
     <t xml:space="preserve">ЧАД</t>
@@ -1587,7 +1593,10 @@
     <t xml:space="preserve">ШВЕЦИЯ</t>
   </si>
   <si>
-    <t xml:space="preserve">ШРИ-ЛАНКА</t>
+    <t xml:space="preserve">ШПИЦБЕРГЕН И ЯН-МАЙЕН</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ШРИ ЛАНКА</t>
   </si>
   <si>
     <t xml:space="preserve">ЭКВАДОР</t>
@@ -1608,7 +1617,10 @@
     <t xml:space="preserve">ЮЖНАЯ АФРИКА</t>
   </si>
   <si>
-    <t xml:space="preserve">ЮЖНАЯ ДЖОРДЖИЯ И ЮЖНЫЕ САНДВИЧЕВЫЕ ОСТРОВА</t>
+    <t xml:space="preserve">ЮЖНАЯ ГЕОРГИЯ И ЮЖНЫЕ САНДВИЧЕВЫ ОСТРОВА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ЮЖНАЯ ОСЕТИЯ</t>
   </si>
   <si>
     <t xml:space="preserve">ЯМАЙКА</t>
@@ -3136,7 +3148,7 @@
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="66.34"/>
@@ -32408,11 +32420,11 @@
   </sheetPr>
   <dimension ref="A1:I246"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E217" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50"/>
@@ -34332,16 +34344,24 @@
       </c>
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H240" s="27"/>
+      <c r="H240" s="27" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H241" s="27"/>
+      <c r="H241" s="27" t="s">
+        <v>530</v>
+      </c>
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H242" s="27"/>
+      <c r="H242" s="27" t="s">
+        <v>531</v>
+      </c>
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H243" s="27"/>
+      <c r="H243" s="27" t="s">
+        <v>532</v>
+      </c>
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H244" s="27"/>
@@ -34380,7 +34400,7 @@
       <selection pane="topLeft" activeCell="B58" activeCellId="0" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.76"/>
@@ -34388,10 +34408,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
-        <v>529</v>
+        <v>533</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34399,7 +34419,7 @@
         <v>4203</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>531</v>
+        <v>535</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34407,7 +34427,7 @@
         <v>4203100001</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34415,7 +34435,7 @@
         <v>4203100009</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34423,7 +34443,7 @@
         <v>6106</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34431,7 +34451,7 @@
         <v>6106100000</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>535</v>
+        <v>539</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34439,7 +34459,7 @@
         <v>6106200000</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34447,7 +34467,7 @@
         <v>6106901000</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>537</v>
+        <v>541</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34455,7 +34475,7 @@
         <v>6106903000</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>538</v>
+        <v>542</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34463,7 +34483,7 @@
         <v>6106905000</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34471,7 +34491,7 @@
         <v>6106909000</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34479,7 +34499,7 @@
         <v>6201</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>541</v>
+        <v>545</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34487,7 +34507,7 @@
         <v>6201200000</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>542</v>
+        <v>546</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34495,7 +34515,7 @@
         <v>6201300000</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34503,7 +34523,7 @@
         <v>6201400000</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>544</v>
+        <v>548</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34511,7 +34531,7 @@
         <v>6201900000</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34519,7 +34539,7 @@
         <v>6202</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34527,7 +34547,7 @@
         <v>6202200000</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>547</v>
+        <v>551</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34535,7 +34555,7 @@
         <v>6202300000</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34543,7 +34563,7 @@
         <v>6202400001</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34551,7 +34571,7 @@
         <v>6202400009</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34559,7 +34579,7 @@
         <v>6202900001</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>551</v>
+        <v>555</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34567,7 +34587,7 @@
         <v>6202900009</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>552</v>
+        <v>556</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34575,7 +34595,7 @@
         <v>6302</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>553</v>
+        <v>557</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34583,7 +34603,7 @@
         <v>6302100001</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>554</v>
+        <v>558</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34591,7 +34611,7 @@
         <v>6302100009</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34599,7 +34619,7 @@
         <v>6302210000</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>556</v>
+        <v>560</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34607,7 +34627,7 @@
         <v>6302221000</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34615,7 +34635,7 @@
         <v>6302229000</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>558</v>
+        <v>562</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34623,7 +34643,7 @@
         <v>6302310001</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34631,7 +34651,7 @@
         <v>6302310009</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34639,7 +34659,7 @@
         <v>6302321000</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34647,7 +34667,7 @@
         <v>6302329000</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34655,7 +34675,7 @@
         <v>6302392001</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34663,7 +34683,7 @@
         <v>6302392009</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34671,7 +34691,7 @@
         <v>6302399000</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34679,7 +34699,7 @@
         <v>6302400000</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>566</v>
+        <v>570</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34687,7 +34707,7 @@
         <v>6302510001</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>567</v>
+        <v>571</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34695,7 +34715,7 @@
         <v>6302510009</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>568</v>
+        <v>572</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34703,7 +34723,7 @@
         <v>6302531000</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34711,7 +34731,7 @@
         <v>6302539000</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>570</v>
+        <v>574</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34719,7 +34739,7 @@
         <v>6302591000</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34727,7 +34747,7 @@
         <v>6302599000</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>572</v>
+        <v>576</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34735,7 +34755,7 @@
         <v>6302600000</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>573</v>
+        <v>577</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34743,7 +34763,7 @@
         <v>6302910000</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>574</v>
+        <v>578</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34751,7 +34771,7 @@
         <v>6302931000</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>575</v>
+        <v>579</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34759,7 +34779,7 @@
         <v>6302939000</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>576</v>
+        <v>580</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34767,7 +34787,7 @@
         <v>6302991000</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>577</v>
+        <v>581</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34775,7 +34795,7 @@
         <v>6302999000</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>578</v>
+        <v>582</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34783,7 +34803,7 @@
         <v>4303</v>
       </c>
       <c r="B50" s="33" t="s">
-        <v>579</v>
+        <v>583</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34791,7 +34811,7 @@
         <v>4303109010</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>580</v>
+        <v>584</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34799,7 +34819,7 @@
         <v>4303109020</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34807,7 +34827,7 @@
         <v>4303109030</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34815,7 +34835,7 @@
         <v>4303109040</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>583</v>
+        <v>587</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34823,7 +34843,7 @@
         <v>4303109050</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>584</v>
+        <v>588</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34831,7 +34851,7 @@
         <v>4303109060</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>585</v>
+        <v>589</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34839,7 +34859,7 @@
         <v>4303109080</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>586</v>
+        <v>590</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34847,7 +34867,7 @@
         <v>3303</v>
       </c>
       <c r="B58" s="35" t="s">
-        <v>587</v>
+        <v>591</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34855,7 +34875,7 @@
         <v>3303001000</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>588</v>
+        <v>592</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34863,7 +34883,7 @@
         <v>3303009000</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>589</v>
+        <v>593</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34871,7 +34891,7 @@
         <v>4011</v>
       </c>
       <c r="B61" s="33" t="s">
-        <v>590</v>
+        <v>594</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34879,7 +34899,7 @@
         <v>4011100003</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>591</v>
+        <v>595</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34887,7 +34907,7 @@
         <v>4011100009</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>592</v>
+        <v>596</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34895,7 +34915,7 @@
         <v>4011201000</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>593</v>
+        <v>597</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34903,7 +34923,7 @@
         <v>4011209000</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34911,7 +34931,7 @@
         <v>4011400000</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>595</v>
+        <v>599</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34919,7 +34939,7 @@
         <v>4011700000</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34927,7 +34947,7 @@
         <v>4011800000</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>597</v>
+        <v>601</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34935,7 +34955,7 @@
         <v>4011900000</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34943,7 +34963,7 @@
         <v>6401</v>
       </c>
       <c r="B70" s="33" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34951,7 +34971,7 @@
         <v>6401100000</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34959,7 +34979,7 @@
         <v>6401921000</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>601</v>
+        <v>605</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34967,7 +34987,7 @@
         <v>6401929000</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34975,7 +34995,7 @@
         <v>6401990000</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>603</v>
+        <v>607</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34983,7 +35003,7 @@
         <v>6402</v>
       </c>
       <c r="B75" s="33" t="s">
-        <v>604</v>
+        <v>608</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34991,7 +35011,7 @@
         <v>6402121000</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>605</v>
+        <v>609</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34999,7 +35019,7 @@
         <v>6402129000</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>606</v>
+        <v>610</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35007,7 +35027,7 @@
         <v>6402190000</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>607</v>
+        <v>611</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35015,7 +35035,7 @@
         <v>6402200000</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>608</v>
+        <v>612</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35023,7 +35043,7 @@
         <v>6402911000</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>609</v>
+        <v>613</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="26.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35031,7 +35051,7 @@
         <v>6402919000</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>610</v>
+        <v>614</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35039,7 +35059,7 @@
         <v>6402990500</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>611</v>
+        <v>615</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35047,7 +35067,7 @@
         <v>6402991000</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>612</v>
+        <v>616</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35055,7 +35075,7 @@
         <v>6402993100</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>613</v>
+        <v>617</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35063,7 +35083,7 @@
         <v>6402993900</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35071,7 +35091,7 @@
         <v>6402995000</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>615</v>
+        <v>619</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35079,7 +35099,7 @@
         <v>6402999100</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35087,7 +35107,7 @@
         <v>6402999300</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35095,7 +35115,7 @@
         <v>6402999600</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35103,7 +35123,7 @@
         <v>6402999800</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35111,7 +35131,7 @@
         <v>6403</v>
       </c>
       <c r="B91" s="33" t="s">
-        <v>619</v>
+        <v>623</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35119,7 +35139,7 @@
         <v>6403120000</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>620</v>
+        <v>624</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35127,7 +35147,7 @@
         <v>6403190000</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>621</v>
+        <v>625</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35135,7 +35155,7 @@
         <v>6403200000</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>622</v>
+        <v>626</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35143,7 +35163,7 @@
         <v>6403400000</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="52.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35151,7 +35171,7 @@
         <v>6403510500</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>624</v>
+        <v>628</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35159,7 +35179,7 @@
         <v>6403511100</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>625</v>
+        <v>629</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35167,7 +35187,7 @@
         <v>6403511500</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>626</v>
+        <v>630</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35175,7 +35195,7 @@
         <v>6403511900</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>627</v>
+        <v>631</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35183,7 +35203,7 @@
         <v>6403519100</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>628</v>
+        <v>632</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35191,7 +35211,7 @@
         <v>6403519500</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35199,7 +35219,7 @@
         <v>6403519900</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>630</v>
+        <v>634</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35207,7 +35227,7 @@
         <v>6403590500</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35215,7 +35235,7 @@
         <v>6403591100</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>632</v>
+        <v>636</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35223,7 +35243,7 @@
         <v>6403593100</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35231,7 +35251,7 @@
         <v>6403593500</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35239,7 +35259,7 @@
         <v>6403593900</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>635</v>
+        <v>639</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35247,7 +35267,7 @@
         <v>6403595000</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>636</v>
+        <v>640</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35255,7 +35275,7 @@
         <v>6403599100</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>637</v>
+        <v>641</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35263,7 +35283,7 @@
         <v>6403599500</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35271,7 +35291,7 @@
         <v>6403599900</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35279,7 +35299,7 @@
         <v>6403910500</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>640</v>
+        <v>644</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35287,7 +35307,7 @@
         <v>6403911100</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>641</v>
+        <v>645</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35295,7 +35315,7 @@
         <v>6403911300</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>642</v>
+        <v>646</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35303,7 +35323,7 @@
         <v>6403911600</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35311,7 +35331,7 @@
         <v>6403911800</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35319,7 +35339,7 @@
         <v>6403919100</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>645</v>
+        <v>649</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35327,7 +35347,7 @@
         <v>6403919300</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>646</v>
+        <v>650</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35335,7 +35355,7 @@
         <v>6403919600</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35343,7 +35363,7 @@
         <v>6403919800</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>648</v>
+        <v>652</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35351,7 +35371,7 @@
         <v>6403990500</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>649</v>
+        <v>653</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35359,7 +35379,7 @@
         <v>6403991100</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>650</v>
+        <v>654</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35367,7 +35387,7 @@
         <v>6403993100</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>651</v>
+        <v>655</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35375,7 +35395,7 @@
         <v>6403993300</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>652</v>
+        <v>656</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35383,7 +35403,7 @@
         <v>6403993600</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>653</v>
+        <v>657</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35391,7 +35411,7 @@
         <v>6403993800</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>654</v>
+        <v>658</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35399,7 +35419,7 @@
         <v>6403995000</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>655</v>
+        <v>659</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35407,7 +35427,7 @@
         <v>6403999100</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>656</v>
+        <v>660</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35415,7 +35435,7 @@
         <v>6403999300</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>657</v>
+        <v>661</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35423,7 +35443,7 @@
         <v>6403999600</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>658</v>
+        <v>662</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35431,7 +35451,7 @@
         <v>6403999800</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>659</v>
+        <v>663</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35439,7 +35459,7 @@
         <v>6404</v>
       </c>
       <c r="B132" s="33" t="s">
-        <v>660</v>
+        <v>664</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35447,7 +35467,7 @@
         <v>6404110000</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35455,7 +35475,7 @@
         <v>6404191000</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>662</v>
+        <v>666</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35463,7 +35483,7 @@
         <v>6404199000</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>663</v>
+        <v>667</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35471,7 +35491,7 @@
         <v>6404191000</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>664</v>
+        <v>668</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35479,7 +35499,7 @@
         <v>6404209000</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>665</v>
+        <v>669</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35487,7 +35507,7 @@
         <v>6405</v>
       </c>
       <c r="B138" s="33" t="s">
-        <v>666</v>
+        <v>670</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35495,7 +35515,7 @@
         <v>6405100001</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>667</v>
+        <v>671</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35503,7 +35523,7 @@
         <v>6405100009</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>668</v>
+        <v>672</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35511,7 +35531,7 @@
         <v>6405201000</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>669</v>
+        <v>673</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35519,7 +35539,7 @@
         <v>6405209100</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>670</v>
+        <v>674</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35527,7 +35547,7 @@
         <v>6405209900</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>671</v>
+        <v>675</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35535,7 +35555,7 @@
         <v>6405901000</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>672</v>
+        <v>676</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35543,7 +35563,7 @@
         <v>6405909000</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>673</v>
+        <v>677</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrections: - countries edit
</commit_message>
<xml_diff>
--- a/app/download_dir/белье_по каждому размеру.xlsx
+++ b/app/download_dir/белье_по каждому размеру.xlsx
@@ -1161,7 +1161,7 @@
     <t xml:space="preserve">СЕРЫЙ/ЗЕЛЕНЫЙ</t>
   </si>
   <si>
-    <t xml:space="preserve">КОРЕЯ, ДЕМОКРАТИЧЕСКАЯ НАРОДНАЯ РЕСПУБЛИКА</t>
+    <t xml:space="preserve">СЕВЕРНАЯ КОРЕЯ</t>
   </si>
   <si>
     <t xml:space="preserve">СИНЕ-ЗЕЛЕНЫЙ</t>
@@ -1395,7 +1395,7 @@
     <t xml:space="preserve">РЕСПУБЛИКА КОНГО</t>
   </si>
   <si>
-    <t xml:space="preserve">РЕСПУБЛИКА КОРЕЯ</t>
+    <t xml:space="preserve">ЮЖНАЯ КОРЕЯ</t>
   </si>
   <si>
     <t xml:space="preserve">РЕСПУБЛИКА МАКЕДОНИЯ, БЫВШАЯ ЮГОСЛАВСКАЯ РЕСПУБЛИКА</t>
@@ -1467,7 +1467,7 @@
     <t xml:space="preserve">СЛОВЕНИЯ</t>
   </si>
   <si>
-    <t xml:space="preserve">СОЕДИНЕННЫЕ ШТАТЫ</t>
+    <t xml:space="preserve">США</t>
   </si>
   <si>
     <t xml:space="preserve">СОЛОМОНОВЫ ОСТРОВА</t>
@@ -3148,7 +3148,7 @@
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="66.34"/>
@@ -32420,11 +32420,11 @@
   </sheetPr>
   <dimension ref="A1:I246"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50"/>
@@ -34400,7 +34400,7 @@
       <selection pane="topLeft" activeCell="B58" activeCellId="0" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.76"/>

</xml_diff>

<commit_message>
Corrections: - promo message - countries list edited
</commit_message>
<xml_diff>
--- a/app/download_dir/белье_по каждому размеру.xlsx
+++ b/app/download_dir/белье_по каждому размеру.xlsx
@@ -579,7 +579,7 @@
     <t xml:space="preserve">МИКРОФИБРА</t>
   </si>
   <si>
-    <t xml:space="preserve">БЕЛОРУССИЯ</t>
+    <t xml:space="preserve">РЕСПУБЛИКА БЕЛАРУСЬ</t>
   </si>
   <si>
     <t xml:space="preserve">КОМПЛЕКТ СТОЛОВОГО БЕЛЬЯ</t>
@@ -3144,11 +3144,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ1732"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O8" activeCellId="0" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="66.34"/>
@@ -32361,7 +32361,7 @@
     <mergeCell ref="C5:K5"/>
     <mergeCell ref="P6:R6"/>
   </mergeCells>
-  <dataValidations count="10">
+  <dataValidations count="11">
     <dataValidation allowBlank="true" errorStyle="stop" operator="lessThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B7:B1606 M7:M1606" type="textLength">
       <formula1>129</formula1>
       <formula2>0</formula2>
@@ -32375,7 +32375,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="O1199:O1606" type="list">
-      <formula1>Справочники!$H$2:$H$245</formula1>
+      <formula1>Справочники!$H$2:$H$243</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I7:I1606" type="list">
@@ -32390,8 +32390,8 @@
       <formula1>Справочники!$D$2:$D$32</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="O7:O1198" type="list">
-      <formula1>Справочники!$H$2:$H$246</formula1>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="O8:O1198" type="list">
+      <formula1>Справочники!$H$2:$H$244</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="P7:P1732" type="list">
@@ -32400,6 +32400,10 @@
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G7:G1658" type="list">
       <formula1>Справочники!$E$3:$E$112</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="O7" type="list">
+      <formula1>Справочники!$H$2:$H$242</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -32418,13 +32422,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I246"/>
+  <dimension ref="A1:I244"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G148" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H170" activeCellId="0" sqref="H170"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H165" activeCellId="0" sqref="H165"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50"/>
@@ -34365,12 +34369,6 @@
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H244" s="27"/>
-    </row>
-    <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H245" s="27"/>
-    </row>
-    <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H246" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -34396,11 +34394,11 @@
   </sheetPr>
   <dimension ref="A1:B145"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A127" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A127" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B58" activeCellId="0" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.76"/>

</xml_diff>

<commit_message>
Corrections: - countries list edit
</commit_message>
<xml_diff>
--- a/app/download_dir/белье_по каждому размеру.xlsx
+++ b/app/download_dir/белье_по каждому размеру.xlsx
@@ -579,7 +579,7 @@
     <t xml:space="preserve">МИКРОФИБРА</t>
   </si>
   <si>
-    <t xml:space="preserve">РЕСПУБЛИКА БЕЛАРУСЬ</t>
+    <t xml:space="preserve">БЕЛОРУССИЯ</t>
   </si>
   <si>
     <t xml:space="preserve">КОМПЛЕКТ СТОЛОВОГО БЕЛЬЯ</t>
@@ -3148,7 +3148,7 @@
       <selection pane="topLeft" activeCell="O8" activeCellId="0" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="66.34"/>
@@ -32425,10 +32425,10 @@
   <dimension ref="A1:I244"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H165" activeCellId="0" sqref="H165"/>
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50"/>
@@ -34398,7 +34398,7 @@
       <selection pane="topLeft" activeCell="B58" activeCellId="0" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.76"/>

</xml_diff>

<commit_message>
Corrections: - linen types edit
</commit_message>
<xml_diff>
--- a/app/download_dir/белье_по каждому размеру.xlsx
+++ b/app/download_dir/белье_по каждому размеру.xlsx
@@ -411,7 +411,7 @@
     <t xml:space="preserve">АНГОЛА</t>
   </si>
   <si>
-    <t xml:space="preserve">КОМПЛЕКТ</t>
+    <t xml:space="preserve">КОМПЛЕКТ ПОСТЕЛЬНОГО БЕЛЬЯ</t>
   </si>
   <si>
     <t xml:space="preserve">БИРЮЗОВЫЙ</t>
@@ -3148,7 +3148,7 @@
       <selection pane="topLeft" activeCell="O8" activeCellId="0" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="66.34"/>
@@ -32424,11 +32424,11 @@
   </sheetPr>
   <dimension ref="A1:I244"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50"/>
@@ -34398,7 +34398,7 @@
       <selection pane="topLeft" activeCell="B58" activeCellId="0" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.76"/>

</xml_diff>